<commit_message>
reworked examples and anova
</commit_message>
<xml_diff>
--- a/data/flea_dog_cat_fox.xlsx
+++ b/data/flea_dog_cat_fox.xlsx
@@ -627,7 +627,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="n">
-        <v>12.1</v>
+        <v>7.7</v>
       </c>
       <c r="C16" t="n">
         <v>21</v>
@@ -644,7 +644,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="n">
-        <v>13.2</v>
+        <v>8.1</v>
       </c>
       <c r="C17" t="n">
         <v>25</v>
@@ -661,7 +661,7 @@
         <v>7</v>
       </c>
       <c r="B18" t="n">
-        <v>14.1</v>
+        <v>9.1</v>
       </c>
       <c r="C18" t="n">
         <v>31</v>
@@ -712,7 +712,7 @@
         <v>7</v>
       </c>
       <c r="B21" t="n">
-        <v>11.5</v>
+        <v>8.6</v>
       </c>
       <c r="C21" t="n">
         <v>18</v>
@@ -729,7 +729,7 @@
         <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>10.8</v>
+        <v>10.3</v>
       </c>
       <c r="C22" t="n">
         <v>19</v>

</xml_diff>